<commit_message>
Get invoice products for orders (#558)
* Refactored GrandeDolceIntegrationService

1. Put invoice products to order instead of order products

* Removed unnecessary comments

* Disabled GrandeDolceIntegrationServiceITest

* Added product amount counting

* Test fixing

* Fixed comment NPE into DeliveryTimeRangeParser

* HotFix

---------

Co-authored-by: Taras Orlovskyi <taras.orlovskyi@nordstrom.com>
</commit_message>
<xml_diff>
--- a/goods-partner-backend/src/main/resources/report/template_car_load_protocol.xlsx
+++ b/goods-partner-backend/src/main/resources/report/template_car_load_protocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my\projects\GoodsPartner\GoodsPartner\goods-partner-backend\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7ADE8E-F056-48B5-A7F0-8E3249FEDA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5BA2A8-55F1-4182-BE8C-A4DD9EEBCC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AB3F32B7-11D8-469F-AD07-BE6B95A3F998}"/>
   </bookViews>
@@ -38,13 +38,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Кількість</t>
-  </si>
-  <si>
     <t>Номенклатура/Контрагент/Документ /Вантажоодержувач/Адреса</t>
   </si>
   <si>
     <t>Всього в од.вимір.</t>
+  </si>
+  <si>
+    <t>Кількість упак.</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,7 +540,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,13 +556,13 @@
     </row>
     <row r="2" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -589,15 +589,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100082AD486D4940F4DB5EFD1F02C4E6F07" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c696f3a61c0835f11669c57fcff420eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="41b742d8-69b9-4ba8-a131-5a619b071b4b" xmlns:ns4="9db58efd-4e74-45e5-ab40-f5b9c8d1f931" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="033edba951a6612f633ee413b9911643" ns3:_="" ns4:_="">
     <xsd:import namespace="41b742d8-69b9-4ba8-a131-5a619b071b4b"/>
@@ -800,6 +791,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -809,14 +809,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F04B9D57-78CB-4C1B-A289-2BF25F1D358C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7786CF82-489C-405B-BC80-C5BBF21037E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -835,6 +827,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F04B9D57-78CB-4C1B-A289-2BF25F1D358C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAE5B8E7-54FF-4E77-8EFE-FE4DB6B2D62F}">
   <ds:schemaRefs>

</xml_diff>